<commit_message>
Test for variable substitution
</commit_message>
<xml_diff>
--- a/src/xlsx_extract/test_data/source.xlsx
+++ b/src/xlsx_extract/test_data/source.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maraspeli/Build/Python/xlsx-extract/src/xlsx_extract/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077859CA-36DE-8C43-919D-DD537CF759FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{077859CA-36DE-8C43-919D-DD537CF759FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2BE5884-D45C-7048-B7AF-4DF0840ABF0F}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="37560" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t>Plan</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>output</t>
   </si>
 </sst>
 </file>
@@ -531,15 +543,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3CB2ACF-D95E-3340-AEE4-CC6F43CEB251}">
-  <dimension ref="B3:F9"/>
+  <dimension ref="B3:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.35546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
@@ -630,6 +642,22 @@
       </c>
       <c r="F9">
         <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -642,13 +670,13 @@
   <dimension ref="B4:H13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:H8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.89453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.35546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
@@ -821,10 +849,10 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection sqref="A1:E5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>

</xml_diff>